<commit_message>
Location geändert, zwei Beispiel-TaxiStands eingefügt
</commit_message>
<xml_diff>
--- a/IT-Projekt/database/data_v1.xlsx
+++ b/IT-Projekt/database/data_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Desktop\IT-Projekt-Anylogic\IT-Projekt\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B40E88-08FB-4E6A-AA1E-03B855258D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1752D42-4BFC-44D2-B9E7-2D02562C6BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50085" yWindow="6885" windowWidth="16920" windowHeight="10830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15675" yWindow="6645" windowWidth="16920" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,139 +442,139 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2">
-        <v>48.142536026787603</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C2" s="2">
-        <v>11.558612949515201</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D2" s="2">
-        <v>48.142536026787603</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E2" s="2">
-        <v>11.4639759376253</v>
+        <v>9.7309718027690906</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C3" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D3" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E3" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C4" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D4" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E4" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C5" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D5" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E5" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C6" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D6" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E6" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C7" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D7" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E7" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C8" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D8" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E8" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B9" s="2">
-        <v>48.177299528963502</v>
+        <v>52.375394479042797</v>
       </c>
       <c r="C9" s="2">
-        <v>11.570040636965601</v>
+        <v>9.7315180260351593</v>
       </c>
       <c r="D9" s="2">
-        <v>48.177316544815703</v>
+        <v>52.382591097574597</v>
       </c>
       <c r="E9" s="2">
-        <v>11.5595018616942</v>
+        <v>9.7309718027690906</v>
       </c>
     </row>
   </sheetData>
@@ -588,7 +588,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,10 +615,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>48.146137193358001</v>
+        <v>52.381989108834198</v>
       </c>
       <c r="B2" s="2">
-        <v>11.465264577216599</v>
+        <v>9.7381182223916092</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>48.180130507890098</v>
+        <v>52.375468581529297</v>
       </c>
       <c r="B3" s="2">
-        <v>11.570917662658699</v>
+        <v>9.7509848120552896</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C51E590-80CB-4323-97E0-0D589D623D52}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,10 +687,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>48.180130507890098</v>
+        <v>52.381989108834198</v>
       </c>
       <c r="B2" s="2">
-        <v>11.6009176626587</v>
+        <v>9.7401182223916098</v>
       </c>
       <c r="D2">
         <v>30000</v>

</xml_diff>

<commit_message>
* Koordinaten des Zentrums angepasst * 20 neue Taxistände eingepflegt
</commit_message>
<xml_diff>
--- a/IT-Projekt/database/data_v1.xlsx
+++ b/IT-Projekt/database/data_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Desktop\IT-Projekt-Anylogic\IT-Projekt\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1752D42-4BFC-44D2-B9E7-2D02562C6BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F68FBE-039B-46BE-8A43-BE94E6505B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15675" yWindow="6645" windowWidth="16920" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -411,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -585,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6468AD4D-C8E8-46B8-9DA3-61897E2D91EC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,37 +616,428 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>52.381989108834198</v>
-      </c>
-      <c r="B2" s="2">
-        <v>9.7381182223916092</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>100</v>
-      </c>
-      <c r="E2">
+      <c r="A2" s="4">
+        <v>52.386400000000002</v>
+      </c>
+      <c r="B2" s="4">
+        <v>9.7109100000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>52.375468581529297</v>
-      </c>
-      <c r="B3" s="2">
-        <v>9.7509848120552896</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
+      <c r="A3" s="4">
+        <v>52.389690000000002</v>
+      </c>
+      <c r="B3" s="4">
+        <v>9.7207399999999993</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>100</v>
+      </c>
+      <c r="E3" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>52.381039999999999</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9.7362800000000007</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>52.37323</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9.72865</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>52.373089999999998</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9.7082700000000006</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>100</v>
+      </c>
+      <c r="E6" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>52.380740000000003</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.6991599999999991</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>52.366759999999999</v>
+      </c>
+      <c r="B8" s="4">
+        <v>9.7177699999999998</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>52.373089999999998</v>
+      </c>
+      <c r="B9" s="4">
+        <v>9.7440700000000007</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>52.390889999999999</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9.7360600000000002</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>100</v>
+      </c>
+      <c r="E10" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>52.397959999999998</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9.7083300000000001</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>200</v>
+      </c>
+      <c r="E11" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>52.374769999999998</v>
+      </c>
+      <c r="B12" s="4">
+        <v>9.6938300000000002</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>200</v>
+      </c>
+      <c r="E12" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>52.365789999999997</v>
+      </c>
+      <c r="B13" s="4">
+        <v>9.7010799999999993</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>200</v>
+      </c>
+      <c r="E13" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>52.364780000000003</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9.7360000000000007</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>200</v>
+      </c>
+      <c r="E14" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>52.37377</v>
+      </c>
+      <c r="B15" s="4">
+        <v>9.7597199999999997</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>200</v>
+      </c>
+      <c r="E15" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>52.386130000000001</v>
+      </c>
+      <c r="B16" s="4">
+        <v>9.7498400000000007</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>200</v>
+      </c>
+      <c r="E16" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>52.399000000000001</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9.7409400000000002</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>200</v>
+      </c>
+      <c r="E17" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>52.366669999999999</v>
+      </c>
+      <c r="B18" s="4">
+        <v>9.6840899999999994</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>200</v>
+      </c>
+      <c r="E18" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>52.359400000000001</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9.7108000000000008</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>200</v>
+      </c>
+      <c r="E19" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>52.364429999999999</v>
+      </c>
+      <c r="B20" s="4">
+        <v>9.7525899999999996</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>52.381419999999999</v>
+      </c>
+      <c r="B21" s="4">
+        <v>9.7661999999999995</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+      <c r="E21" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>52.356819999999999</v>
+      </c>
+      <c r="B22" s="4">
+        <v>9.76</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>200</v>
+      </c>
+      <c r="E22" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>52.365400000000001</v>
+      </c>
+      <c r="B23" s="4">
+        <v>9.7692200000000007</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>200</v>
+      </c>
+      <c r="E23" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>52.349710000000002</v>
+      </c>
+      <c r="B24" s="4">
+        <v>9.7695500000000006</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>200</v>
+      </c>
+      <c r="E24" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>52.399050000000003</v>
+      </c>
+      <c r="B25" s="4">
+        <v>9.7587399999999995</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>200</v>
+      </c>
+      <c r="E25" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>52.397950000000002</v>
+      </c>
+      <c r="B26" s="4">
+        <v>9.7270000000000003</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>200</v>
+      </c>
+      <c r="E26" s="3">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transport von bis zu 4 Personen eingefügt
</commit_message>
<xml_diff>
--- a/IT-Projekt/database/data_v1.xlsx
+++ b/IT-Projekt/database/data_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Desktop\IT-Projekt-Anylogic\IT-Projekt\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F68FBE-039B-46BE-8A43-BE94E6505B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCC37E7-1231-4BDC-8B1B-95ED35427879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Tesla</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +579,150 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>120</v>
+      </c>
+      <c r="B10" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D10" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E10" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>120</v>
+      </c>
+      <c r="B11" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D11" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>120</v>
+      </c>
+      <c r="B12" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D12" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E12" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>120</v>
+      </c>
+      <c r="B13" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D13" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E13" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>120</v>
+      </c>
+      <c r="B14" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C14" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D14" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E14" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>120</v>
+      </c>
+      <c r="B15" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C15" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D15" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E15" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>120</v>
+      </c>
+      <c r="B16" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C16" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D16" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E16" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>120</v>
+      </c>
+      <c r="B17" s="4">
+        <v>52.375394479042797</v>
+      </c>
+      <c r="C17" s="4">
+        <v>9.7315180260351593</v>
+      </c>
+      <c r="D17" s="4">
+        <v>52.382591097574597</v>
+      </c>
+      <c r="E17" s="4">
+        <v>9.7309718027690906</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -589,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6468AD4D-C8E8-46B8-9DA3-61897E2D91EC}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C51E590-80CB-4323-97E0-0D589D623D52}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,6 +1242,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>52.389690000000002</v>
+      </c>
+      <c r="B3" s="4">
+        <v>9.7207399999999993</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+      <c r="E3">
+        <v>30000</v>
+      </c>
+      <c r="F3">
+        <v>30000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>